<commit_message>
Fixed Cumulative Harvest Data
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Gliricidia/Observed.xlsx
+++ b/Tests/UnderReview/Gliricidia/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Gliricidia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Tests\UnderReview\Gliricidia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A73D73-C173-4F49-A488-DAFC0E0B9B2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8558C8D-FFE6-49C7-9705-F4E860C411BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedSoil" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="67">
   <si>
     <t>Year</t>
   </si>
@@ -230,6 +232,9 @@
   </si>
   <si>
     <t>Maize.Grain.Number</t>
+  </si>
+  <si>
+    <t>CuttingManagement.Script.CumulativeTotalRemovalWt</t>
   </si>
 </sst>
 </file>
@@ -3862,16 +3867,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>232410</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>537210</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3898,16 +3903,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>293370</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>598170</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3934,16 +3939,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>156210</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>461010</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5149,10 +5154,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4410" topLeftCell="L1" activePane="topRight"/>
+      <selection activeCell="A27" sqref="A27"/>
+      <selection pane="topRight" activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5168,9 +5173,12 @@
     <col min="12" max="12" width="19.15625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.68359375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.68359375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.68359375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.41796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5231,8 +5239,11 @@
       <c r="T1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5258,7 +5269,7 @@
         <v>279.06976744186045</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -5284,7 +5295,7 @@
         <v>418.60465116279073</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -5310,7 +5321,7 @@
         <v>395.34883720930236</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -5336,7 +5347,7 @@
         <v>511.62790697674421</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -5362,7 +5373,7 @@
         <v>558.1395348837209</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -5388,7 +5399,7 @@
         <v>581.39534883720933</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -5414,7 +5425,7 @@
         <v>651.16279069767438</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -5440,7 +5451,7 @@
         <v>348.83720930232556</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -5466,7 +5477,7 @@
         <v>488.37209302325584</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -5492,7 +5503,7 @@
         <v>534.88372093023258</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -5512,7 +5523,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -5538,7 +5549,7 @@
         <v>1.4229359211203001</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -5564,7 +5575,7 @@
         <v>4.5519769090135398</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -5590,7 +5601,7 @@
         <v>6.9641670285147903</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -5616,7 +5627,7 @@
         <v>9.2473239917054801</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -5642,7 +5653,7 @@
         <v>9.9534090444337906</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -5668,7 +5679,7 @@
         <v>6.3154613715885803</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5694,7 +5705,7 @@
         <v>9.1720363768313895</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -5720,7 +5731,7 @@
         <v>12.9463057989389</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -5743,7 +5754,7 @@
         <v>4.4524590163934405</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -5766,7 +5777,7 @@
         <v>4.0852459016393396</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -5789,7 +5800,7 @@
         <v>3.5147540983606493</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -5812,7 +5823,7 @@
         <v>3.1475409836065498</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -5835,7 +5846,7 @@
         <v>2.97049180327868</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -5858,7 +5869,7 @@
         <v>2.9639344262295002</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -5890,8 +5901,12 @@
         <f t="shared" ref="T27:T36" si="5">R27+S27</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U27">
+        <f>T27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -5923,8 +5938,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U28">
+        <f>T28+U27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -5956,8 +5975,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U29">
+        <f t="shared" ref="U29:U92" si="6">T29+U28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -5989,8 +6012,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6022,8 +6049,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -6055,8 +6086,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -6077,8 +6112,12 @@
         <f t="shared" si="5"/>
         <v>1702</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U33">
+        <f t="shared" si="6"/>
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -6088,7 +6127,7 @@
       <c r="D34" s="2"/>
       <c r="F34" s="1"/>
       <c r="H34">
-        <f t="shared" ref="H34:H78" si="6">L34+M34</f>
+        <f t="shared" ref="H34:H78" si="7">L34+M34</f>
         <v>61.705824595829014</v>
       </c>
       <c r="L34">
@@ -6110,8 +6149,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U34">
+        <f>T34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -6121,7 +6164,7 @@
       <c r="D35" s="2"/>
       <c r="F35" s="1"/>
       <c r="H35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>332.61875882103914</v>
       </c>
       <c r="L35">
@@ -6143,8 +6186,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -6154,7 +6201,7 @@
       <c r="D36" s="2"/>
       <c r="F36" s="1"/>
       <c r="H36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>820.84815187646734</v>
       </c>
       <c r="L36">
@@ -6176,8 +6223,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -6187,7 +6238,7 @@
       <c r="D37" s="2"/>
       <c r="F37" s="1"/>
       <c r="H37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L37">
@@ -6211,8 +6262,12 @@
         <f>R37+S37</f>
         <v>820.84815187646734</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U37">
+        <f t="shared" si="6"/>
+        <v>820.84815187646734</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -6222,7 +6277,7 @@
       <c r="D38" s="2"/>
       <c r="F38" s="1"/>
       <c r="H38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>165.40720438167909</v>
       </c>
       <c r="L38">
@@ -6241,11 +6296,15 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <f t="shared" ref="T38:T101" si="7">R38+S38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="T38:T101" si="8">R38+S38</f>
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="6"/>
+        <v>820.84815187646734</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -6255,7 +6314,7 @@
       <c r="D39" s="2"/>
       <c r="F39" s="1"/>
       <c r="H39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>379.74879132764863</v>
       </c>
       <c r="L39">
@@ -6274,11 +6333,15 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="6"/>
+        <v>820.84815187646734</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -6288,7 +6351,7 @@
       <c r="D40" s="2"/>
       <c r="F40" s="1"/>
       <c r="H40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>323.61428149007526</v>
       </c>
       <c r="L40">
@@ -6307,11 +6370,15 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="6"/>
+        <v>820.84815187646734</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -6329,11 +6396,15 @@
         <v>570.06274117537123</v>
       </c>
       <c r="T41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>624.15184812353266</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U41">
+        <f t="shared" si="6"/>
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -6343,7 +6414,7 @@
       <c r="D42" s="2"/>
       <c r="F42" s="1"/>
       <c r="H42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12.03896761729743</v>
       </c>
       <c r="L42">
@@ -6362,11 +6433,15 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <f>T42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -6376,7 +6451,7 @@
       <c r="D43" s="2"/>
       <c r="F43" s="1"/>
       <c r="H43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>179.01911469563191</v>
       </c>
       <c r="L43">
@@ -6395,11 +6470,15 @@
         <v>0</v>
       </c>
       <c r="T43">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -6409,7 +6488,7 @@
       <c r="D44" s="2"/>
       <c r="F44" s="1"/>
       <c r="H44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>74.618089574231959</v>
       </c>
       <c r="L44">
@@ -6430,11 +6509,15 @@
         <v>58.224163027656672</v>
       </c>
       <c r="T44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>104.40102512139995</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U44">
+        <f t="shared" si="6"/>
+        <v>104.40102512139995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -6444,7 +6527,7 @@
       <c r="D45" s="2"/>
       <c r="F45" s="1"/>
       <c r="H45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>240.24832019553577</v>
       </c>
       <c r="L45">
@@ -6463,11 +6546,15 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="6"/>
+        <v>104.40102512139995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -6475,7 +6562,7 @@
         <v>35291</v>
       </c>
       <c r="H46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>105.48595827699356</v>
       </c>
       <c r="L46">
@@ -6496,11 +6583,15 @@
         <v>91.495113329174757</v>
       </c>
       <c r="T46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>134.76236191854221</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U46">
+        <f t="shared" si="6"/>
+        <v>239.16338703994217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -6508,7 +6599,7 @@
         <v>35347</v>
       </c>
       <c r="H47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>211.90609310432478</v>
       </c>
       <c r="L47">
@@ -6527,11 +6618,15 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="6"/>
+        <v>239.16338703994217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -6539,7 +6634,7 @@
         <v>35348</v>
       </c>
       <c r="H48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43.849221260747726</v>
       </c>
       <c r="L48">
@@ -6560,8 +6655,12 @@
         <v>124.76606363069239</v>
       </c>
       <c r="T48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>168.05687184357706</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="6"/>
+        <v>407.22025888351925</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -6572,7 +6671,7 @@
         <v>35399</v>
       </c>
       <c r="H49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>251.04458013543194</v>
       </c>
       <c r="L49">
@@ -6591,8 +6690,12 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="6"/>
+        <v>407.22025888351925</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -6603,7 +6706,7 @@
         <v>35400</v>
       </c>
       <c r="H50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>94.531923815290298</v>
       </c>
       <c r="L50">
@@ -6624,8 +6727,12 @@
         <v>124.76606363069288</v>
       </c>
       <c r="T50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>156.51265632014164</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="6"/>
+        <v>563.73291520366092</v>
       </c>
       <c r="W50">
         <v>0.3</v>
@@ -6639,7 +6746,7 @@
         <v>35461</v>
       </c>
       <c r="H51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56.347601536630819</v>
       </c>
       <c r="L51">
@@ -6658,8 +6765,12 @@
         <v>33.27095030151763</v>
       </c>
       <c r="T51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>56.347601536630819</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="6"/>
+        <v>620.08051674029173</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -6685,14 +6796,18 @@
         <v>29.477646080265686</v>
       </c>
       <c r="T52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36.919483259708329</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="6"/>
+        <v>657</v>
       </c>
       <c r="V52">
         <v>2</v>
       </c>
       <c r="W52">
-        <f t="shared" ref="W52:W59" si="8">1-EXP(-W$50*V52)</f>
+        <f t="shared" ref="W52:W59" si="9">1-EXP(-W$50*V52)</f>
         <v>0.45118836390597361</v>
       </c>
     </row>
@@ -6704,7 +6819,7 @@
         <v>35215.666701388887</v>
       </c>
       <c r="H53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
       <c r="L53">
@@ -6726,14 +6841,18 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <f>T53</f>
         <v>0</v>
       </c>
       <c r="V53">
         <v>3</v>
       </c>
       <c r="W53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.59343034025940078</v>
       </c>
     </row>
@@ -6745,7 +6864,7 @@
         <v>35271.333402777775</v>
       </c>
       <c r="H54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>319</v>
       </c>
       <c r="L54">
@@ -6767,14 +6886,18 @@
         <v>0</v>
       </c>
       <c r="T54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V54">
         <v>4</v>
       </c>
       <c r="W54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.69880578808779781</v>
       </c>
     </row>
@@ -6786,7 +6909,7 @@
         <v>35327.000104166669</v>
       </c>
       <c r="H55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>722</v>
       </c>
       <c r="L55">
@@ -6808,14 +6931,18 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V55">
         <v>5</v>
       </c>
       <c r="W55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.77686983985157021</v>
       </c>
     </row>
@@ -6827,7 +6954,7 @@
         <v>35387.666805555556</v>
       </c>
       <c r="H56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1302</v>
       </c>
       <c r="L56">
@@ -6849,14 +6976,18 @@
         <v>0</v>
       </c>
       <c r="T56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V56">
         <v>6</v>
       </c>
       <c r="W56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.83470111177841344</v>
       </c>
     </row>
@@ -6868,7 +6999,7 @@
         <v>35439.333500000008</v>
       </c>
       <c r="H57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1043</v>
       </c>
       <c r="L57">
@@ -6890,14 +7021,18 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V57">
         <v>7</v>
       </c>
       <c r="W57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.87754357174701814</v>
       </c>
     </row>
@@ -6909,7 +7044,7 @@
         <v>35499.000196759262</v>
       </c>
       <c r="H58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1431</v>
       </c>
       <c r="L58">
@@ -6931,14 +7066,18 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U58">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V58">
         <v>8</v>
       </c>
       <c r="W58">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.90928204671058754</v>
       </c>
     </row>
@@ -6962,14 +7101,18 @@
         <v>1398</v>
       </c>
       <c r="T59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>1431</v>
+      </c>
+      <c r="U59">
+        <f t="shared" si="6"/>
         <v>1431</v>
       </c>
       <c r="V59">
         <v>9</v>
       </c>
       <c r="W59">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.93279448726025027</v>
       </c>
     </row>
@@ -6981,7 +7124,7 @@
         <v>35215.666701388887</v>
       </c>
       <c r="H60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>138</v>
       </c>
       <c r="L60">
@@ -7003,7 +7146,11 @@
         <v>0</v>
       </c>
       <c r="T60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <f>T60</f>
         <v>0</v>
       </c>
     </row>
@@ -7015,7 +7162,7 @@
         <v>35271.333402777775</v>
       </c>
       <c r="H61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>371</v>
       </c>
       <c r="L61">
@@ -7037,7 +7184,11 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7049,7 +7200,7 @@
         <v>35326.000100000005</v>
       </c>
       <c r="H62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>682</v>
       </c>
       <c r="L62">
@@ -7077,7 +7228,11 @@
         <v>0</v>
       </c>
       <c r="T62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7089,7 +7244,7 @@
         <v>35327.000104166669</v>
       </c>
       <c r="H63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L63">
@@ -7113,7 +7268,11 @@
         <v>415.99999999999994</v>
       </c>
       <c r="T63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>679</v>
+      </c>
+      <c r="U63">
+        <f t="shared" si="6"/>
         <v>679</v>
       </c>
     </row>
@@ -7125,7 +7284,7 @@
         <v>35387.666805555556</v>
       </c>
       <c r="H64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>151</v>
       </c>
       <c r="L64">
@@ -7147,11 +7306,15 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <f t="shared" si="6"/>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -7159,7 +7322,7 @@
         <v>35439.333500000008</v>
       </c>
       <c r="H65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>347</v>
       </c>
       <c r="L65">
@@ -7181,11 +7344,15 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <f t="shared" si="6"/>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>61</v>
       </c>
@@ -7193,7 +7360,7 @@
         <v>35499.000196759262</v>
       </c>
       <c r="H66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>978</v>
       </c>
       <c r="L66">
@@ -7215,11 +7382,15 @@
         <v>692</v>
       </c>
       <c r="T66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>978</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U66">
+        <f t="shared" si="6"/>
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>61</v>
       </c>
@@ -7235,11 +7406,15 @@
         <v>5</v>
       </c>
       <c r="T67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U67">
+        <f t="shared" si="6"/>
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>62</v>
       </c>
@@ -7247,7 +7422,7 @@
         <v>35215.667002314818</v>
       </c>
       <c r="H68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>166</v>
       </c>
       <c r="L68">
@@ -7275,11 +7450,15 @@
         <v>0</v>
       </c>
       <c r="T68">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U68">
+        <f>T68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>62</v>
       </c>
@@ -7287,7 +7466,7 @@
         <v>35216.667002314818</v>
       </c>
       <c r="H69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
       <c r="L69">
@@ -7311,11 +7490,15 @@
         <v>17</v>
       </c>
       <c r="T69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U69">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>62</v>
       </c>
@@ -7323,7 +7506,7 @@
         <v>35271.334004629629</v>
       </c>
       <c r="H70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>385</v>
       </c>
       <c r="L70">
@@ -7351,11 +7534,15 @@
         <v>0</v>
       </c>
       <c r="T70">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -7363,7 +7550,7 @@
         <v>35272.334004629629</v>
       </c>
       <c r="H71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>246</v>
       </c>
       <c r="L71">
@@ -7387,11 +7574,15 @@
         <v>60</v>
       </c>
       <c r="T71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>139</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U71">
+        <f t="shared" si="6"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>62</v>
       </c>
@@ -7399,7 +7590,7 @@
         <v>35326.001000000004</v>
       </c>
       <c r="H72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>478</v>
       </c>
       <c r="L72">
@@ -7427,11 +7618,15 @@
         <v>0</v>
       </c>
       <c r="T72">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U72">
+        <f t="shared" si="6"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -7439,7 +7634,7 @@
         <v>35327.001000000004</v>
       </c>
       <c r="H73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>261</v>
       </c>
       <c r="L73">
@@ -7463,11 +7658,15 @@
         <v>125</v>
       </c>
       <c r="T73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>217</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U73">
+        <f t="shared" si="6"/>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>62</v>
       </c>
@@ -7475,7 +7674,7 @@
         <v>35387.667997685188</v>
       </c>
       <c r="H74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>549</v>
       </c>
       <c r="L74">
@@ -7503,11 +7702,15 @@
         <v>0</v>
       </c>
       <c r="T74">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U74">
+        <f t="shared" si="6"/>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -7515,7 +7718,7 @@
         <v>35388.667997685188</v>
       </c>
       <c r="H75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>327</v>
       </c>
       <c r="L75">
@@ -7539,11 +7742,15 @@
         <v>146</v>
       </c>
       <c r="T75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>222</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U75">
+        <f t="shared" si="6"/>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>62</v>
       </c>
@@ -7551,7 +7758,7 @@
         <v>35439.335000000006</v>
       </c>
       <c r="H76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>254</v>
       </c>
       <c r="L76">
@@ -7579,11 +7786,15 @@
         <v>0</v>
       </c>
       <c r="T76">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <f t="shared" si="6"/>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -7591,7 +7802,7 @@
         <v>35440.335000000006</v>
       </c>
       <c r="H77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>95</v>
       </c>
       <c r="L77">
@@ -7615,11 +7826,15 @@
         <v>107</v>
       </c>
       <c r="T77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U77">
+        <f t="shared" si="6"/>
+        <v>805</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>62</v>
       </c>
@@ -7627,7 +7842,7 @@
         <v>35499.002002314817</v>
       </c>
       <c r="H78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
       <c r="L78">
@@ -7649,11 +7864,15 @@
         <v>138</v>
       </c>
       <c r="T78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U78">
+        <f t="shared" si="6"/>
+        <v>997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>62</v>
       </c>
@@ -7669,11 +7888,15 @@
         <v>-7</v>
       </c>
       <c r="T79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-11</v>
       </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U79">
+        <f t="shared" si="6"/>
+        <v>986</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>41</v>
       </c>
@@ -7695,11 +7918,15 @@
         <v>152</v>
       </c>
       <c r="T80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>179</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U80">
+        <f>T80</f>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>41</v>
       </c>
@@ -7714,11 +7941,15 @@
         <v>0</v>
       </c>
       <c r="T81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U81">
+        <f t="shared" si="6"/>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -7734,11 +7965,15 @@
         <v>0</v>
       </c>
       <c r="T82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U82">
+        <f t="shared" si="6"/>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>41</v>
       </c>
@@ -7754,11 +7989,15 @@
         <v>243</v>
       </c>
       <c r="T83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>266</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U83">
+        <f t="shared" si="6"/>
+        <v>678</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>41</v>
       </c>
@@ -7780,11 +8019,15 @@
         <v>0</v>
       </c>
       <c r="T84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>215</v>
       </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U84">
+        <f t="shared" si="6"/>
+        <v>893</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -7804,11 +8047,15 @@
         <v>0</v>
       </c>
       <c r="T85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U85">
+        <f t="shared" si="6"/>
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>41</v>
       </c>
@@ -7828,11 +8075,15 @@
         <v>141</v>
       </c>
       <c r="T86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U86">
+        <f t="shared" si="6"/>
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>41</v>
       </c>
@@ -7852,11 +8103,15 @@
         <v>0</v>
       </c>
       <c r="T87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>175</v>
       </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U87">
+        <f t="shared" si="6"/>
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>41</v>
       </c>
@@ -7876,11 +8131,15 @@
         <v>0</v>
       </c>
       <c r="T88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U88">
+        <f t="shared" si="6"/>
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>41</v>
       </c>
@@ -7900,11 +8159,15 @@
         <v>136</v>
       </c>
       <c r="T89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>265</v>
       </c>
-    </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U89">
+        <f t="shared" si="6"/>
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -7924,11 +8187,15 @@
         <v>0</v>
       </c>
       <c r="T90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>214</v>
       </c>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U90">
+        <f t="shared" si="6"/>
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>41</v>
       </c>
@@ -7948,11 +8215,15 @@
         <v>0</v>
       </c>
       <c r="T91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U91">
+        <f t="shared" si="6"/>
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -7972,11 +8243,15 @@
         <v>142</v>
       </c>
       <c r="T92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>309</v>
       </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U92">
+        <f t="shared" si="6"/>
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>41</v>
       </c>
@@ -7996,11 +8271,15 @@
         <v>0</v>
       </c>
       <c r="T93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>250</v>
       </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U93">
+        <f t="shared" ref="U93:U128" si="10">T93+U92</f>
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>41</v>
       </c>
@@ -8020,11 +8299,15 @@
         <v>0</v>
       </c>
       <c r="T94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>155</v>
       </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U94">
+        <f t="shared" si="10"/>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>41</v>
       </c>
@@ -8044,11 +8327,15 @@
         <v>209</v>
       </c>
       <c r="T95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>209</v>
       </c>
-    </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U95">
+        <f t="shared" si="10"/>
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>41</v>
       </c>
@@ -8068,11 +8355,15 @@
         <v>0</v>
       </c>
       <c r="T96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315</v>
       </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U96">
+        <f t="shared" si="10"/>
+        <v>3374</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>41</v>
       </c>
@@ -8092,11 +8383,15 @@
         <v>0</v>
       </c>
       <c r="T97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>195</v>
       </c>
-    </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U97">
+        <f t="shared" si="10"/>
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>41</v>
       </c>
@@ -8116,11 +8411,15 @@
         <v>0</v>
       </c>
       <c r="T98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>182</v>
       </c>
-    </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U98">
+        <f t="shared" si="10"/>
+        <v>3751</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>41</v>
       </c>
@@ -8140,11 +8439,15 @@
         <v>335</v>
       </c>
       <c r="T99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>335</v>
       </c>
-    </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U99">
+        <f t="shared" si="10"/>
+        <v>4086</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>41</v>
       </c>
@@ -8164,11 +8467,15 @@
         <v>0</v>
       </c>
       <c r="T100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
-    </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U100">
+        <f t="shared" si="10"/>
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>41</v>
       </c>
@@ -8188,11 +8495,15 @@
         <v>0</v>
       </c>
       <c r="T101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U101">
+        <f t="shared" si="10"/>
+        <v>4506</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>41</v>
       </c>
@@ -8212,11 +8523,15 @@
         <v>0</v>
       </c>
       <c r="T102">
-        <f t="shared" ref="T102:T128" si="9">R102+S102</f>
+        <f t="shared" ref="T102:T128" si="11">R102+S102</f>
         <v>148</v>
       </c>
-    </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U102">
+        <f t="shared" si="10"/>
+        <v>4654</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>41</v>
       </c>
@@ -8236,11 +8551,15 @@
         <v>340</v>
       </c>
       <c r="T103">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>340</v>
       </c>
-    </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U103">
+        <f t="shared" si="10"/>
+        <v>4994</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>41</v>
       </c>
@@ -8260,11 +8579,15 @@
         <v>0</v>
       </c>
       <c r="T104">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>210</v>
       </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U104">
+        <f t="shared" si="10"/>
+        <v>5204</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>41</v>
       </c>
@@ -8284,11 +8607,15 @@
         <v>0</v>
       </c>
       <c r="T105">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U105">
+        <f t="shared" si="10"/>
+        <v>5312</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>41</v>
       </c>
@@ -8308,11 +8635,15 @@
         <v>0</v>
       </c>
       <c r="T106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U106">
+        <f t="shared" si="10"/>
+        <v>5419</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>41</v>
       </c>
@@ -8332,11 +8663,15 @@
         <v>450</v>
       </c>
       <c r="T107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>451</v>
       </c>
-    </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U107">
+        <f t="shared" si="10"/>
+        <v>5870</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>41</v>
       </c>
@@ -8356,11 +8691,15 @@
         <v>0</v>
       </c>
       <c r="T108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>277</v>
       </c>
-    </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U108">
+        <f t="shared" si="10"/>
+        <v>6147</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>41</v>
       </c>
@@ -8380,11 +8719,15 @@
         <v>0</v>
       </c>
       <c r="T109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142</v>
       </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U109">
+        <f t="shared" si="10"/>
+        <v>6289</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>41</v>
       </c>
@@ -8404,11 +8747,15 @@
         <v>0</v>
       </c>
       <c r="T110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142</v>
       </c>
-    </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U110">
+        <f t="shared" si="10"/>
+        <v>6431</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>41</v>
       </c>
@@ -8428,11 +8775,15 @@
         <v>400</v>
       </c>
       <c r="T111">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U111">
+        <f t="shared" si="10"/>
+        <v>6831</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>41</v>
       </c>
@@ -8453,11 +8804,15 @@
         <v>0</v>
       </c>
       <c r="T112">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>240.52626000000001</v>
       </c>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U112">
+        <f t="shared" si="10"/>
+        <v>7071.5262599999996</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>41</v>
       </c>
@@ -8478,11 +8833,15 @@
         <v>0</v>
       </c>
       <c r="T113">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>122.73768</v>
       </c>
-    </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U113">
+        <f t="shared" si="10"/>
+        <v>7194.2639399999998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>41</v>
       </c>
@@ -8503,11 +8862,15 @@
         <v>0</v>
       </c>
       <c r="T114">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>122.73768</v>
       </c>
-    </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U114">
+        <f t="shared" si="10"/>
+        <v>7317.00162</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>41</v>
       </c>
@@ -8527,11 +8890,15 @@
         <v>400</v>
       </c>
       <c r="T115">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U115">
+        <f t="shared" si="10"/>
+        <v>7717.00162</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>41</v>
       </c>
@@ -8551,11 +8918,15 @@
         <v>0</v>
       </c>
       <c r="T116">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>243</v>
       </c>
-    </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U116">
+        <f t="shared" si="10"/>
+        <v>7960.00162</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>41</v>
       </c>
@@ -8575,11 +8946,15 @@
         <v>0</v>
       </c>
       <c r="T117">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>124</v>
       </c>
-    </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U117">
+        <f t="shared" si="10"/>
+        <v>8084.00162</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>41</v>
       </c>
@@ -8599,11 +8974,15 @@
         <v>0</v>
       </c>
       <c r="T118">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>124</v>
       </c>
-    </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U118">
+        <f t="shared" si="10"/>
+        <v>8208.0016199999991</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>41</v>
       </c>
@@ -8625,11 +9004,15 @@
         <v>123.7</v>
       </c>
       <c r="T119">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>223.7</v>
       </c>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U119">
+        <f t="shared" si="10"/>
+        <v>8431.7016199999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>41</v>
       </c>
@@ -8651,11 +9034,15 @@
         <v>0</v>
       </c>
       <c r="T120">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U120">
+        <f t="shared" si="10"/>
+        <v>8574.7016199999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>41</v>
       </c>
@@ -8677,11 +9064,15 @@
         <v>0</v>
       </c>
       <c r="T121">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>104.4</v>
       </c>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U121">
+        <f t="shared" si="10"/>
+        <v>8679.1016199999995</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>41</v>
       </c>
@@ -8703,11 +9094,15 @@
         <v>0</v>
       </c>
       <c r="T122">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>91.49</v>
       </c>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U122">
+        <f t="shared" si="10"/>
+        <v>8770.5916199999992</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>41</v>
       </c>
@@ -8729,11 +9124,15 @@
         <v>157.16999999999999</v>
       </c>
       <c r="T123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>240.01</v>
       </c>
-    </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U123">
+        <f t="shared" si="10"/>
+        <v>9010.6016199999995</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>41</v>
       </c>
@@ -8755,11 +9154,15 @@
         <v>0</v>
       </c>
       <c r="T124">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>70.237837648793089</v>
       </c>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U124">
+        <f t="shared" si="10"/>
+        <v>9080.8394576487917</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>41</v>
       </c>
@@ -8781,11 +9184,15 @@
         <v>0</v>
       </c>
       <c r="T125">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>51.24</v>
       </c>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U125">
+        <f t="shared" si="10"/>
+        <v>9132.0794576487915</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>41</v>
       </c>
@@ -8807,11 +9214,15 @@
         <v>365.41529860520842</v>
       </c>
       <c r="T126">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>528.12849133511952</v>
       </c>
-    </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U126">
+        <f t="shared" si="10"/>
+        <v>9660.2079489839107</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>41</v>
       </c>
@@ -8833,11 +9244,15 @@
         <v>0</v>
       </c>
       <c r="T127">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>131.4</v>
       </c>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="U127">
+        <f t="shared" si="10"/>
+        <v>9791.6079489839103</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>41</v>
       </c>
@@ -8859,8 +9274,12 @@
         <v>0</v>
       </c>
       <c r="T128">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>132.5</v>
+      </c>
+      <c r="U128">
+        <f t="shared" si="10"/>
+        <v>9924.1079489839103</v>
       </c>
     </row>
   </sheetData>
@@ -8874,7 +9293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added sensibility test and cleaned up biomass removal data
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Gliricidia/Observed.xlsx
+++ b/Tests/UnderReview/Gliricidia/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Tests\UnderReview\Gliricidia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8558C8D-FFE6-49C7-9705-F4E860C411BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D58795B-F744-427A-97CA-6F7209AED77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5154,9 +5154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4410" topLeftCell="L1" activePane="topRight"/>
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="6900" topLeftCell="N1" activePane="topRight"/>
+      <selection activeCell="F81" sqref="F81"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
@@ -5627,7 +5627,7 @@
         <v>9.2473239917054801</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>9.9534090444337906</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>6.3154613715885803</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>9.1720363768313895</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>12.9463057989389</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>4.4524590163934405</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>4.0852459016393396</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>3.5147540983606493</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>3.1475409836065498</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>2.97049180327868</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>2.9639344262295002</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -5901,12 +5901,8 @@
         <f t="shared" ref="T27:T36" si="5">R27+S27</f>
         <v>0</v>
       </c>
-      <c r="U27">
-        <f>T27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -5938,12 +5934,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U28">
-        <f>T28+U27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -5975,12 +5967,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U29">
-        <f t="shared" ref="U29:U92" si="6">T29+U28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -6012,12 +6000,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U30">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6049,12 +6033,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U31">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -6086,10 +6066,6 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
@@ -6113,7 +6089,6 @@
         <v>1702</v>
       </c>
       <c r="U33">
-        <f t="shared" si="6"/>
         <v>1702</v>
       </c>
     </row>
@@ -6127,7 +6102,7 @@
       <c r="D34" s="2"/>
       <c r="F34" s="1"/>
       <c r="H34">
-        <f t="shared" ref="H34:H78" si="7">L34+M34</f>
+        <f t="shared" ref="H34:H78" si="6">L34+M34</f>
         <v>61.705824595829014</v>
       </c>
       <c r="L34">
@@ -6147,10 +6122,6 @@
       </c>
       <c r="T34">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U34">
-        <f>T34</f>
         <v>0</v>
       </c>
     </row>
@@ -6164,7 +6135,7 @@
       <c r="D35" s="2"/>
       <c r="F35" s="1"/>
       <c r="H35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>332.61875882103914</v>
       </c>
       <c r="L35">
@@ -6184,10 +6155,6 @@
       </c>
       <c r="T35">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U35">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -6201,7 +6168,7 @@
       <c r="D36" s="2"/>
       <c r="F36" s="1"/>
       <c r="H36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>820.84815187646734</v>
       </c>
       <c r="L36">
@@ -6221,10 +6188,6 @@
       </c>
       <c r="T36">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -6238,7 +6201,7 @@
       <c r="D37" s="2"/>
       <c r="F37" s="1"/>
       <c r="H37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L37">
@@ -6263,7 +6226,6 @@
         <v>820.84815187646734</v>
       </c>
       <c r="U37">
-        <f t="shared" si="6"/>
         <v>820.84815187646734</v>
       </c>
     </row>
@@ -6277,7 +6239,7 @@
       <c r="D38" s="2"/>
       <c r="F38" s="1"/>
       <c r="H38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>165.40720438167909</v>
       </c>
       <c r="L38">
@@ -6296,12 +6258,8 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <f t="shared" ref="T38:T101" si="8">R38+S38</f>
-        <v>0</v>
-      </c>
-      <c r="U38">
-        <f t="shared" si="6"/>
-        <v>820.84815187646734</v>
+        <f t="shared" ref="T38:T101" si="7">R38+S38</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6314,7 +6272,7 @@
       <c r="D39" s="2"/>
       <c r="F39" s="1"/>
       <c r="H39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>379.74879132764863</v>
       </c>
       <c r="L39">
@@ -6333,12 +6291,8 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U39">
-        <f t="shared" si="6"/>
-        <v>820.84815187646734</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6351,7 +6305,7 @@
       <c r="D40" s="2"/>
       <c r="F40" s="1"/>
       <c r="H40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>323.61428149007526</v>
       </c>
       <c r="L40">
@@ -6370,12 +6324,8 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U40">
-        <f t="shared" si="6"/>
-        <v>820.84815187646734</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6396,11 +6346,10 @@
         <v>570.06274117537123</v>
       </c>
       <c r="T41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>624.15184812353266</v>
       </c>
       <c r="U41">
-        <f t="shared" si="6"/>
         <v>1445</v>
       </c>
     </row>
@@ -6414,7 +6363,7 @@
       <c r="D42" s="2"/>
       <c r="F42" s="1"/>
       <c r="H42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>12.03896761729743</v>
       </c>
       <c r="L42">
@@ -6433,11 +6382,7 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U42">
-        <f>T42</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6451,7 +6396,7 @@
       <c r="D43" s="2"/>
       <c r="F43" s="1"/>
       <c r="H43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>179.01911469563191</v>
       </c>
       <c r="L43">
@@ -6470,11 +6415,7 @@
         <v>0</v>
       </c>
       <c r="T43">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6488,7 +6429,7 @@
       <c r="D44" s="2"/>
       <c r="F44" s="1"/>
       <c r="H44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>74.618089574231959</v>
       </c>
       <c r="L44">
@@ -6509,11 +6450,10 @@
         <v>58.224163027656672</v>
       </c>
       <c r="T44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>104.40102512139995</v>
       </c>
       <c r="U44">
-        <f t="shared" si="6"/>
         <v>104.40102512139995</v>
       </c>
     </row>
@@ -6527,7 +6467,7 @@
       <c r="D45" s="2"/>
       <c r="F45" s="1"/>
       <c r="H45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>240.24832019553577</v>
       </c>
       <c r="L45">
@@ -6546,12 +6486,8 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U45">
-        <f t="shared" si="6"/>
-        <v>104.40102512139995</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6562,7 +6498,7 @@
         <v>35291</v>
       </c>
       <c r="H46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>105.48595827699356</v>
       </c>
       <c r="L46">
@@ -6583,11 +6519,10 @@
         <v>91.495113329174757</v>
       </c>
       <c r="T46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>134.76236191854221</v>
       </c>
       <c r="U46">
-        <f t="shared" si="6"/>
         <v>239.16338703994217</v>
       </c>
     </row>
@@ -6599,7 +6534,7 @@
         <v>35347</v>
       </c>
       <c r="H47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>211.90609310432478</v>
       </c>
       <c r="L47">
@@ -6618,12 +6553,8 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U47">
-        <f t="shared" si="6"/>
-        <v>239.16338703994217</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6634,7 +6565,7 @@
         <v>35348</v>
       </c>
       <c r="H48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>43.849221260747726</v>
       </c>
       <c r="L48">
@@ -6655,11 +6586,10 @@
         <v>124.76606363069239</v>
       </c>
       <c r="T48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>168.05687184357706</v>
       </c>
       <c r="U48">
-        <f t="shared" si="6"/>
         <v>407.22025888351925</v>
       </c>
     </row>
@@ -6671,7 +6601,7 @@
         <v>35399</v>
       </c>
       <c r="H49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>251.04458013543194</v>
       </c>
       <c r="L49">
@@ -6690,12 +6620,8 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="6"/>
-        <v>407.22025888351925</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -6706,7 +6632,7 @@
         <v>35400</v>
       </c>
       <c r="H50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>94.531923815290298</v>
       </c>
       <c r="L50">
@@ -6727,11 +6653,10 @@
         <v>124.76606363069288</v>
       </c>
       <c r="T50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>156.51265632014164</v>
       </c>
       <c r="U50">
-        <f t="shared" si="6"/>
         <v>563.73291520366092</v>
       </c>
       <c r="W50">
@@ -6746,30 +6671,29 @@
         <v>35461</v>
       </c>
       <c r="H51">
+        <f t="shared" si="6"/>
+        <v>56.347601536630819</v>
+      </c>
+      <c r="L51">
+        <v>23.076651235113193</v>
+      </c>
+      <c r="M51">
+        <v>33.27095030151763</v>
+      </c>
+      <c r="N51">
+        <v>28.848758996831151</v>
+      </c>
+      <c r="R51">
+        <v>23.076651235113193</v>
+      </c>
+      <c r="S51">
+        <v>33.27095030151763</v>
+      </c>
+      <c r="T51">
         <f t="shared" si="7"/>
         <v>56.347601536630819</v>
       </c>
-      <c r="L51">
-        <v>23.076651235113193</v>
-      </c>
-      <c r="M51">
-        <v>33.27095030151763</v>
-      </c>
-      <c r="N51">
-        <v>28.848758996831151</v>
-      </c>
-      <c r="R51">
-        <v>23.076651235113193</v>
-      </c>
-      <c r="S51">
-        <v>33.27095030151763</v>
-      </c>
-      <c r="T51">
-        <f t="shared" si="8"/>
-        <v>56.347601536630819</v>
-      </c>
       <c r="U51">
-        <f t="shared" si="6"/>
         <v>620.08051674029173</v>
       </c>
       <c r="V51">
@@ -6796,18 +6720,17 @@
         <v>29.477646080265686</v>
       </c>
       <c r="T52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>36.919483259708329</v>
       </c>
       <c r="U52">
-        <f t="shared" si="6"/>
         <v>657</v>
       </c>
       <c r="V52">
         <v>2</v>
       </c>
       <c r="W52">
-        <f t="shared" ref="W52:W59" si="9">1-EXP(-W$50*V52)</f>
+        <f t="shared" ref="W52:W59" si="8">1-EXP(-W$50*V52)</f>
         <v>0.45118836390597361</v>
       </c>
     </row>
@@ -6819,7 +6742,7 @@
         <v>35215.666701388887</v>
       </c>
       <c r="H53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
       <c r="L53">
@@ -6841,18 +6764,14 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U53">
-        <f>T53</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V53">
         <v>3</v>
       </c>
       <c r="W53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.59343034025940078</v>
       </c>
     </row>
@@ -6864,7 +6783,7 @@
         <v>35271.333402777775</v>
       </c>
       <c r="H54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>319</v>
       </c>
       <c r="L54">
@@ -6886,18 +6805,14 @@
         <v>0</v>
       </c>
       <c r="T54">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V54">
         <v>4</v>
       </c>
       <c r="W54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.69880578808779781</v>
       </c>
     </row>
@@ -6909,7 +6824,7 @@
         <v>35327.000104166669</v>
       </c>
       <c r="H55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>722</v>
       </c>
       <c r="L55">
@@ -6931,18 +6846,14 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V55">
         <v>5</v>
       </c>
       <c r="W55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.77686983985157021</v>
       </c>
     </row>
@@ -6954,7 +6865,7 @@
         <v>35387.666805555556</v>
       </c>
       <c r="H56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1302</v>
       </c>
       <c r="L56">
@@ -6976,18 +6887,14 @@
         <v>0</v>
       </c>
       <c r="T56">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V56">
         <v>6</v>
       </c>
       <c r="W56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.83470111177841344</v>
       </c>
     </row>
@@ -6999,7 +6906,7 @@
         <v>35439.333500000008</v>
       </c>
       <c r="H57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1043</v>
       </c>
       <c r="L57">
@@ -7021,18 +6928,14 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V57">
         <v>7</v>
       </c>
       <c r="W57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.87754357174701814</v>
       </c>
     </row>
@@ -7044,7 +6947,7 @@
         <v>35499.000196759262</v>
       </c>
       <c r="H58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1431</v>
       </c>
       <c r="L58">
@@ -7066,18 +6969,14 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V58">
         <v>8</v>
       </c>
       <c r="W58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.90928204671058754</v>
       </c>
     </row>
@@ -7101,18 +7000,17 @@
         <v>1398</v>
       </c>
       <c r="T59">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1431</v>
       </c>
       <c r="U59">
-        <f t="shared" si="6"/>
         <v>1431</v>
       </c>
       <c r="V59">
         <v>9</v>
       </c>
       <c r="W59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.93279448726025027</v>
       </c>
     </row>
@@ -7124,7 +7022,7 @@
         <v>35215.666701388887</v>
       </c>
       <c r="H60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
       <c r="L60">
@@ -7146,11 +7044,7 @@
         <v>0</v>
       </c>
       <c r="T60">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U60">
-        <f>T60</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7162,7 +7056,7 @@
         <v>35271.333402777775</v>
       </c>
       <c r="H61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>371</v>
       </c>
       <c r="L61">
@@ -7184,11 +7078,7 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7200,7 +7090,7 @@
         <v>35326.000100000005</v>
       </c>
       <c r="H62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>682</v>
       </c>
       <c r="L62">
@@ -7228,11 +7118,7 @@
         <v>0</v>
       </c>
       <c r="T62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7244,7 +7130,7 @@
         <v>35327.000104166669</v>
       </c>
       <c r="H63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L63">
@@ -7268,11 +7154,10 @@
         <v>415.99999999999994</v>
       </c>
       <c r="T63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>679</v>
       </c>
       <c r="U63">
-        <f t="shared" si="6"/>
         <v>679</v>
       </c>
     </row>
@@ -7284,7 +7169,7 @@
         <v>35387.666805555556</v>
       </c>
       <c r="H64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>151</v>
       </c>
       <c r="L64">
@@ -7306,12 +7191,8 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U64">
-        <f t="shared" si="6"/>
-        <v>679</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7322,7 +7203,7 @@
         <v>35439.333500000008</v>
       </c>
       <c r="H65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>347</v>
       </c>
       <c r="L65">
@@ -7344,12 +7225,8 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U65">
-        <f t="shared" si="6"/>
-        <v>679</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7360,33 +7237,32 @@
         <v>35499.000196759262</v>
       </c>
       <c r="H66">
+        <f t="shared" si="6"/>
+        <v>978</v>
+      </c>
+      <c r="L66">
+        <v>286</v>
+      </c>
+      <c r="M66">
+        <v>692</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>286</v>
+      </c>
+      <c r="S66">
+        <v>692</v>
+      </c>
+      <c r="T66">
         <f t="shared" si="7"/>
         <v>978</v>
       </c>
-      <c r="L66">
-        <v>286</v>
-      </c>
-      <c r="M66">
-        <v>692</v>
-      </c>
-      <c r="P66">
-        <v>0</v>
-      </c>
-      <c r="Q66">
-        <v>0</v>
-      </c>
-      <c r="R66">
-        <v>286</v>
-      </c>
-      <c r="S66">
-        <v>692</v>
-      </c>
-      <c r="T66">
-        <f t="shared" si="8"/>
-        <v>978</v>
-      </c>
       <c r="U66">
-        <f t="shared" si="6"/>
         <v>1657</v>
       </c>
     </row>
@@ -7406,11 +7282,10 @@
         <v>5</v>
       </c>
       <c r="T67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="U67">
-        <f t="shared" si="6"/>
         <v>1663</v>
       </c>
     </row>
@@ -7422,7 +7297,7 @@
         <v>35215.667002314818</v>
       </c>
       <c r="H68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>166</v>
       </c>
       <c r="L68">
@@ -7450,11 +7325,7 @@
         <v>0</v>
       </c>
       <c r="T68">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U68">
-        <f>T68</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7466,7 +7337,7 @@
         <v>35216.667002314818</v>
       </c>
       <c r="H69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
       <c r="L69">
@@ -7490,11 +7361,10 @@
         <v>17</v>
       </c>
       <c r="T69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>68</v>
       </c>
       <c r="U69">
-        <f t="shared" si="6"/>
         <v>68</v>
       </c>
     </row>
@@ -7506,7 +7376,7 @@
         <v>35271.334004629629</v>
       </c>
       <c r="H70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>385</v>
       </c>
       <c r="L70">
@@ -7534,12 +7404,8 @@
         <v>0</v>
       </c>
       <c r="T70">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U70">
-        <f t="shared" si="6"/>
-        <v>68</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7550,7 +7416,7 @@
         <v>35272.334004629629</v>
       </c>
       <c r="H71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>246</v>
       </c>
       <c r="L71">
@@ -7574,11 +7440,10 @@
         <v>60</v>
       </c>
       <c r="T71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>139</v>
       </c>
       <c r="U71">
-        <f t="shared" si="6"/>
         <v>207</v>
       </c>
     </row>
@@ -7590,7 +7455,7 @@
         <v>35326.001000000004</v>
       </c>
       <c r="H72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>478</v>
       </c>
       <c r="L72">
@@ -7618,12 +7483,8 @@
         <v>0</v>
       </c>
       <c r="T72">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U72">
-        <f t="shared" si="6"/>
-        <v>207</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7634,7 +7495,7 @@
         <v>35327.001000000004</v>
       </c>
       <c r="H73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>261</v>
       </c>
       <c r="L73">
@@ -7658,11 +7519,10 @@
         <v>125</v>
       </c>
       <c r="T73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="U73">
-        <f t="shared" si="6"/>
         <v>424</v>
       </c>
     </row>
@@ -7674,7 +7534,7 @@
         <v>35387.667997685188</v>
       </c>
       <c r="H74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>549</v>
       </c>
       <c r="L74">
@@ -7702,12 +7562,8 @@
         <v>0</v>
       </c>
       <c r="T74">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U74">
-        <f t="shared" si="6"/>
-        <v>424</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7718,7 +7574,7 @@
         <v>35388.667997685188</v>
       </c>
       <c r="H75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>327</v>
       </c>
       <c r="L75">
@@ -7742,11 +7598,10 @@
         <v>146</v>
       </c>
       <c r="T75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>222</v>
       </c>
       <c r="U75">
-        <f t="shared" si="6"/>
         <v>646</v>
       </c>
     </row>
@@ -7758,7 +7613,7 @@
         <v>35439.335000000006</v>
       </c>
       <c r="H76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>254</v>
       </c>
       <c r="L76">
@@ -7786,12 +7641,8 @@
         <v>0</v>
       </c>
       <c r="T76">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U76">
-        <f t="shared" si="6"/>
-        <v>646</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7802,7 +7653,7 @@
         <v>35440.335000000006</v>
       </c>
       <c r="H77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>95</v>
       </c>
       <c r="L77">
@@ -7826,11 +7677,10 @@
         <v>107</v>
       </c>
       <c r="T77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>159</v>
       </c>
       <c r="U77">
-        <f t="shared" si="6"/>
         <v>805</v>
       </c>
     </row>
@@ -7842,33 +7692,32 @@
         <v>35499.002002314817</v>
       </c>
       <c r="H78">
+        <f t="shared" si="6"/>
+        <v>192</v>
+      </c>
+      <c r="L78">
+        <v>54</v>
+      </c>
+      <c r="M78">
+        <v>138</v>
+      </c>
+      <c r="P78">
+        <v>54</v>
+      </c>
+      <c r="Q78">
+        <v>138</v>
+      </c>
+      <c r="R78">
+        <v>54</v>
+      </c>
+      <c r="S78">
+        <v>138</v>
+      </c>
+      <c r="T78">
         <f t="shared" si="7"/>
         <v>192</v>
       </c>
-      <c r="L78">
-        <v>54</v>
-      </c>
-      <c r="M78">
-        <v>138</v>
-      </c>
-      <c r="P78">
-        <v>54</v>
-      </c>
-      <c r="Q78">
-        <v>138</v>
-      </c>
-      <c r="R78">
-        <v>54</v>
-      </c>
-      <c r="S78">
-        <v>138</v>
-      </c>
-      <c r="T78">
-        <f t="shared" si="8"/>
-        <v>192</v>
-      </c>
       <c r="U78">
-        <f t="shared" si="6"/>
         <v>997</v>
       </c>
     </row>
@@ -7888,11 +7737,10 @@
         <v>-7</v>
       </c>
       <c r="T79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-11</v>
       </c>
       <c r="U79">
-        <f t="shared" si="6"/>
         <v>986</v>
       </c>
     </row>
@@ -7918,11 +7766,7 @@
         <v>152</v>
       </c>
       <c r="T80">
-        <f t="shared" si="8"/>
-        <v>179</v>
-      </c>
-      <c r="U80">
-        <f>T80</f>
+        <f t="shared" si="7"/>
         <v>179</v>
       </c>
     </row>
@@ -7941,12 +7785,8 @@
         <v>0</v>
       </c>
       <c r="T81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>144</v>
-      </c>
-      <c r="U81">
-        <f t="shared" si="6"/>
-        <v>323</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7965,11 +7805,10 @@
         <v>0</v>
       </c>
       <c r="T82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>89</v>
       </c>
       <c r="U82">
-        <f t="shared" si="6"/>
         <v>412</v>
       </c>
     </row>
@@ -7989,12 +7828,8 @@
         <v>243</v>
       </c>
       <c r="T83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>266</v>
-      </c>
-      <c r="U83">
-        <f t="shared" si="6"/>
-        <v>678</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8019,12 +7854,8 @@
         <v>0</v>
       </c>
       <c r="T84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>215</v>
-      </c>
-      <c r="U84">
-        <f t="shared" si="6"/>
-        <v>893</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8047,11 +7878,10 @@
         <v>0</v>
       </c>
       <c r="T85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>133</v>
       </c>
       <c r="U85">
-        <f t="shared" si="6"/>
         <v>1026</v>
       </c>
     </row>
@@ -8075,12 +7905,8 @@
         <v>141</v>
       </c>
       <c r="T86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>216</v>
-      </c>
-      <c r="U86">
-        <f t="shared" si="6"/>
-        <v>1242</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8103,12 +7929,8 @@
         <v>0</v>
       </c>
       <c r="T87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>175</v>
-      </c>
-      <c r="U87">
-        <f t="shared" si="6"/>
-        <v>1417</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8131,11 +7953,10 @@
         <v>0</v>
       </c>
       <c r="T88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>108</v>
       </c>
       <c r="U88">
-        <f t="shared" si="6"/>
         <v>1525</v>
       </c>
     </row>
@@ -8159,12 +7980,8 @@
         <v>136</v>
       </c>
       <c r="T89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>265</v>
-      </c>
-      <c r="U89">
-        <f t="shared" si="6"/>
-        <v>1790</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8187,12 +8004,8 @@
         <v>0</v>
       </c>
       <c r="T90">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>214</v>
-      </c>
-      <c r="U90">
-        <f t="shared" si="6"/>
-        <v>2004</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8215,11 +8028,10 @@
         <v>0</v>
       </c>
       <c r="T91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>132</v>
       </c>
       <c r="U91">
-        <f t="shared" si="6"/>
         <v>2136</v>
       </c>
     </row>
@@ -8243,12 +8055,8 @@
         <v>142</v>
       </c>
       <c r="T92">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>309</v>
-      </c>
-      <c r="U92">
-        <f t="shared" si="6"/>
-        <v>2445</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8271,12 +8079,8 @@
         <v>0</v>
       </c>
       <c r="T93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>250</v>
-      </c>
-      <c r="U93">
-        <f t="shared" ref="U93:U128" si="10">T93+U92</f>
-        <v>2695</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8299,11 +8103,10 @@
         <v>0</v>
       </c>
       <c r="T94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>155</v>
       </c>
       <c r="U94">
-        <f t="shared" si="10"/>
         <v>2850</v>
       </c>
     </row>
@@ -8327,12 +8130,8 @@
         <v>209</v>
       </c>
       <c r="T95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>209</v>
-      </c>
-      <c r="U95">
-        <f t="shared" si="10"/>
-        <v>3059</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8355,12 +8154,8 @@
         <v>0</v>
       </c>
       <c r="T96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>315</v>
-      </c>
-      <c r="U96">
-        <f t="shared" si="10"/>
-        <v>3374</v>
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8383,12 +8178,8 @@
         <v>0</v>
       </c>
       <c r="T97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>195</v>
-      </c>
-      <c r="U97">
-        <f t="shared" si="10"/>
-        <v>3569</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8411,11 +8202,10 @@
         <v>0</v>
       </c>
       <c r="T98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>182</v>
       </c>
       <c r="U98">
-        <f t="shared" si="10"/>
         <v>3751</v>
       </c>
     </row>
@@ -8439,12 +8229,8 @@
         <v>335</v>
       </c>
       <c r="T99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>335</v>
-      </c>
-      <c r="U99">
-        <f t="shared" si="10"/>
-        <v>4086</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8467,12 +8253,8 @@
         <v>0</v>
       </c>
       <c r="T100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>270</v>
-      </c>
-      <c r="U100">
-        <f t="shared" si="10"/>
-        <v>4356</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8495,12 +8277,8 @@
         <v>0</v>
       </c>
       <c r="T101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>150</v>
-      </c>
-      <c r="U101">
-        <f t="shared" si="10"/>
-        <v>4506</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8523,11 +8301,10 @@
         <v>0</v>
       </c>
       <c r="T102">
-        <f t="shared" ref="T102:T128" si="11">R102+S102</f>
+        <f t="shared" ref="T102:T128" si="9">R102+S102</f>
         <v>148</v>
       </c>
       <c r="U102">
-        <f t="shared" si="10"/>
         <v>4654</v>
       </c>
     </row>
@@ -8551,12 +8328,8 @@
         <v>340</v>
       </c>
       <c r="T103">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>340</v>
-      </c>
-      <c r="U103">
-        <f t="shared" si="10"/>
-        <v>4994</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8579,12 +8352,8 @@
         <v>0</v>
       </c>
       <c r="T104">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>210</v>
-      </c>
-      <c r="U104">
-        <f t="shared" si="10"/>
-        <v>5204</v>
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8607,12 +8376,8 @@
         <v>0</v>
       </c>
       <c r="T105">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>108</v>
-      </c>
-      <c r="U105">
-        <f t="shared" si="10"/>
-        <v>5312</v>
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8635,11 +8400,10 @@
         <v>0</v>
       </c>
       <c r="T106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>107</v>
       </c>
       <c r="U106">
-        <f t="shared" si="10"/>
         <v>5419</v>
       </c>
     </row>
@@ -8663,12 +8427,8 @@
         <v>450</v>
       </c>
       <c r="T107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>451</v>
-      </c>
-      <c r="U107">
-        <f t="shared" si="10"/>
-        <v>5870</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8691,12 +8451,8 @@
         <v>0</v>
       </c>
       <c r="T108">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>277</v>
-      </c>
-      <c r="U108">
-        <f t="shared" si="10"/>
-        <v>6147</v>
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8719,12 +8475,8 @@
         <v>0</v>
       </c>
       <c r="T109">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>142</v>
-      </c>
-      <c r="U109">
-        <f t="shared" si="10"/>
-        <v>6289</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8747,11 +8499,10 @@
         <v>0</v>
       </c>
       <c r="T110">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>142</v>
       </c>
       <c r="U110">
-        <f t="shared" si="10"/>
         <v>6431</v>
       </c>
     </row>
@@ -8775,12 +8526,8 @@
         <v>400</v>
       </c>
       <c r="T111">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>400</v>
-      </c>
-      <c r="U111">
-        <f t="shared" si="10"/>
-        <v>6831</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8804,12 +8551,8 @@
         <v>0</v>
       </c>
       <c r="T112">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>240.52626000000001</v>
-      </c>
-      <c r="U112">
-        <f t="shared" si="10"/>
-        <v>7071.5262599999996</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8833,12 +8576,8 @@
         <v>0</v>
       </c>
       <c r="T113">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>122.73768</v>
-      </c>
-      <c r="U113">
-        <f t="shared" si="10"/>
-        <v>7194.2639399999998</v>
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8862,11 +8601,10 @@
         <v>0</v>
       </c>
       <c r="T114">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>122.73768</v>
       </c>
       <c r="U114">
-        <f t="shared" si="10"/>
         <v>7317.00162</v>
       </c>
     </row>
@@ -8890,12 +8628,8 @@
         <v>400</v>
       </c>
       <c r="T115">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>400</v>
-      </c>
-      <c r="U115">
-        <f t="shared" si="10"/>
-        <v>7717.00162</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8918,12 +8652,8 @@
         <v>0</v>
       </c>
       <c r="T116">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>243</v>
-      </c>
-      <c r="U116">
-        <f t="shared" si="10"/>
-        <v>7960.00162</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8946,12 +8676,8 @@
         <v>0</v>
       </c>
       <c r="T117">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>124</v>
-      </c>
-      <c r="U117">
-        <f t="shared" si="10"/>
-        <v>8084.00162</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -8974,11 +8700,10 @@
         <v>0</v>
       </c>
       <c r="T118">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>124</v>
       </c>
       <c r="U118">
-        <f t="shared" si="10"/>
         <v>8208.0016199999991</v>
       </c>
     </row>
@@ -9004,12 +8729,8 @@
         <v>123.7</v>
       </c>
       <c r="T119">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>223.7</v>
-      </c>
-      <c r="U119">
-        <f t="shared" si="10"/>
-        <v>8431.7016199999998</v>
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9034,12 +8755,8 @@
         <v>0</v>
       </c>
       <c r="T120">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>143</v>
-      </c>
-      <c r="U120">
-        <f t="shared" si="10"/>
-        <v>8574.7016199999998</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9064,12 +8781,8 @@
         <v>0</v>
       </c>
       <c r="T121">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>104.4</v>
-      </c>
-      <c r="U121">
-        <f t="shared" si="10"/>
-        <v>8679.1016199999995</v>
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9094,11 +8807,10 @@
         <v>0</v>
       </c>
       <c r="T122">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>91.49</v>
       </c>
       <c r="U122">
-        <f t="shared" si="10"/>
         <v>8770.5916199999992</v>
       </c>
     </row>
@@ -9124,12 +8836,8 @@
         <v>157.16999999999999</v>
       </c>
       <c r="T123">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>240.01</v>
-      </c>
-      <c r="U123">
-        <f t="shared" si="10"/>
-        <v>9010.6016199999995</v>
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9154,12 +8862,8 @@
         <v>0</v>
       </c>
       <c r="T124">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>70.237837648793089</v>
-      </c>
-      <c r="U124">
-        <f t="shared" si="10"/>
-        <v>9080.8394576487917</v>
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9184,11 +8888,10 @@
         <v>0</v>
       </c>
       <c r="T125">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>51.24</v>
       </c>
       <c r="U125">
-        <f t="shared" si="10"/>
         <v>9132.0794576487915</v>
       </c>
     </row>
@@ -9214,12 +8917,8 @@
         <v>365.41529860520842</v>
       </c>
       <c r="T126">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>528.12849133511952</v>
-      </c>
-      <c r="U126">
-        <f t="shared" si="10"/>
-        <v>9660.2079489839107</v>
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9244,12 +8943,8 @@
         <v>0</v>
       </c>
       <c r="T127">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>131.4</v>
-      </c>
-      <c r="U127">
-        <f t="shared" si="10"/>
-        <v>9791.6079489839103</v>
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -9274,11 +8969,10 @@
         <v>0</v>
       </c>
       <c r="T128">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>132.5</v>
       </c>
       <c r="U128">
-        <f t="shared" si="10"/>
         <v>9924.1079489839103</v>
       </c>
     </row>

</xml_diff>